<commit_message>
adding overage learner tab. Change gender labels
</commit_message>
<xml_diff>
--- a/input_tool/edu_table_helper_EN_AFG.xlsx
+++ b/input_tool/edu_table_helper_EN_AFG.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/MSNAEdu/EduAnalysisTool/input_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{061F18F9-EC50-476C-AE2F-DD009B2D4B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{140A1488-850A-4685-AC13-972AD17E1C6C}"/>
+  <xr:revisionPtr revIDLastSave="110" documentId="13_ncr:1_{061F18F9-EC50-476C-AE2F-DD009B2D4B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F275CA0E-E6CE-47BE-BCCC-3476F013CDE2}"/>
   <bookViews>
-    <workbookView xWindow="-19290" yWindow="-3720" windowWidth="19380" windowHeight="11460" activeTab="1" xr2:uid="{AD85D784-B454-4039-8455-21301024D336}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" activeTab="7" xr2:uid="{AD85D784-B454-4039-8455-21301024D336}"/>
   </bookViews>
   <sheets>
     <sheet name="access" sheetId="1" r:id="rId1"/>
-    <sheet name="out_of_school" sheetId="3" r:id="rId2"/>
-    <sheet name="ece" sheetId="4" r:id="rId3"/>
-    <sheet name="level1" sheetId="5" r:id="rId4"/>
-    <sheet name="level2" sheetId="6" r:id="rId5"/>
-    <sheet name="level3" sheetId="7" r:id="rId6"/>
-    <sheet name="level4" sheetId="8" r:id="rId7"/>
+    <sheet name="overage" sheetId="9" r:id="rId2"/>
+    <sheet name="out_of_school" sheetId="3" r:id="rId3"/>
+    <sheet name="ece" sheetId="4" r:id="rId4"/>
+    <sheet name="level1" sheetId="5" r:id="rId5"/>
+    <sheet name="level2" sheetId="6" r:id="rId6"/>
+    <sheet name="level3" sheetId="7" r:id="rId7"/>
+    <sheet name="level4" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="45">
   <si>
     <t>tab</t>
   </si>
@@ -152,12 +153,6 @@
     <t>% of school-aged children of upper secondary school age currently attending  upper secondary school or higher</t>
   </si>
   <si>
-    <t>Female / woman</t>
-  </si>
-  <si>
-    <t>Male / man</t>
-  </si>
-  <si>
     <t>There is a ban preventing child from attending</t>
   </si>
   <si>
@@ -168,6 +163,21 @@
   </si>
   <si>
     <t>No school in the area or school is too far</t>
+  </si>
+  <si>
+    <t>overage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analysis of overage learners </t>
+  </si>
+  <si>
+    <t>Overage learners</t>
+  </si>
+  <si>
+    <t>Girls</t>
+  </si>
+  <si>
+    <t>Boys</t>
   </si>
 </sst>
 </file>
@@ -193,7 +203,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,6 +222,12 @@
         <bgColor rgb="FFFFEFC1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFEFC1"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -225,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -237,6 +253,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -576,7 +595,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C4"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -636,7 +655,7 @@
     </row>
     <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.75">
       <c r="C3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>18</v>
@@ -644,7 +663,7 @@
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.75">
       <c r="C4" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>19</v>
@@ -656,11 +675,93 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F36B93C1-E6B8-4A90-A407-38EEDC988F7A}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="28.86328125" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="5" max="5" width="38.31640625" customWidth="1"/>
+    <col min="6" max="7" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.75">
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.75">
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39444B71-EEA9-4171-A7FB-692AC9A3C4DA}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -711,28 +812,28 @@
         <v>12</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.75">
       <c r="C3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.75">
       <c r="C4" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.75">
       <c r="G5" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.75">
@@ -745,12 +846,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675A8981-F8A2-408A-9A14-DF2744D820F7}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C4"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -808,7 +909,7 @@
     </row>
     <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.75">
       <c r="C3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>24</v>
@@ -816,7 +917,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.75">
       <c r="C4" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -824,12 +925,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A578C6AC-945F-43C7-88F6-0991BAC5AA47}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C4"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -885,15 +986,13 @@
     </row>
     <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.75">
       <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>22</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.75">
       <c r="C4" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -901,12 +1000,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1234059E-FF89-4231-AEDD-537A0FD72374}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C4"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -962,15 +1061,13 @@
     </row>
     <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.75">
       <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>30</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.75">
       <c r="C4" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -978,12 +1075,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF67C88-2243-4200-BD46-1196A6B1AE0E}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C4"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1039,13 +1136,13 @@
     </row>
     <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.75">
       <c r="C3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.75">
       <c r="C4" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1053,12 +1150,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25073DEA-EBA1-4BC2-8E1E-EDCA81A49738}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1114,13 +1211,13 @@
     </row>
     <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.75">
       <c r="C3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.75">
       <c r="C4" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>